<commit_message>
change script structure for multi scenarios
</commit_message>
<xml_diff>
--- a/__cpttime.xlsx
+++ b/__cpttime.xlsx
@@ -122,7 +122,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -141,6 +141,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -151,7 +157,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -197,8 +203,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -240,8 +248,11 @@
     <xf numFmtId="16" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -264,6 +275,7 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -286,6 +298,7 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1074,10 +1087,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Q15"/>
+  <dimension ref="B1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1640,7 +1653,7 @@
       </c>
     </row>
     <row r="13" spans="2:17">
-      <c r="B13" s="5">
+      <c r="B13" s="15">
         <v>42685</v>
       </c>
       <c r="C13" s="1">
@@ -1682,7 +1695,7 @@
       </c>
     </row>
     <row r="14" spans="2:17">
-      <c r="B14" s="5">
+      <c r="B14" s="15">
         <v>42685</v>
       </c>
       <c r="C14" s="1">
@@ -1720,7 +1733,7 @@
       </c>
     </row>
     <row r="15" spans="2:17">
-      <c r="B15" s="5">
+      <c r="B15" s="15">
         <v>42685</v>
       </c>
       <c r="C15" s="1">
@@ -1745,16 +1758,52 @@
         <v>3.4</v>
       </c>
       <c r="J15" s="3">
-        <f t="shared" ref="J15" si="28">F15*E15*G15/H15</f>
+        <f t="shared" ref="J15:J16" si="28">F15*E15*G15/H15</f>
         <v>1</v>
       </c>
       <c r="K15" s="7">
-        <f t="shared" ref="K15" si="29">I15/J15</f>
+        <f t="shared" ref="K15:K16" si="29">I15/J15</f>
         <v>3.4</v>
       </c>
       <c r="L15">
-        <f t="shared" ref="L15" si="30">G15*F15*E15</f>
+        <f t="shared" ref="L15:L16" si="30">G15*F15*E15</f>
         <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17">
+      <c r="B16" s="15">
+        <v>42685</v>
+      </c>
+      <c r="C16" s="1">
+        <v>900</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="E16" s="10">
+        <v>2</v>
+      </c>
+      <c r="F16" s="10">
+        <v>36</v>
+      </c>
+      <c r="G16" s="10">
+        <v>10</v>
+      </c>
+      <c r="H16" s="10">
+        <v>10</v>
+      </c>
+      <c r="I16" s="6"/>
+      <c r="J16" s="3">
+        <f t="shared" si="28"/>
+        <v>72</v>
+      </c>
+      <c r="K16" s="7">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="30"/>
+        <v>720</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor edits on plots
</commit_message>
<xml_diff>
--- a/__cpttime.xlsx
+++ b/__cpttime.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="3020" windowWidth="24140" windowHeight="13340" tabRatio="500"/>
+    <workbookView xWindow="1800" yWindow="7860" windowWidth="24140" windowHeight="13340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -157,8 +157,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -252,7 +254,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -276,6 +278,7 @@
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -299,6 +302,7 @@
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -433,11 +437,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2121396808"/>
-        <c:axId val="2073324040"/>
+        <c:axId val="-2124918152"/>
+        <c:axId val="-2125170248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2121396808"/>
+        <c:axId val="-2124918152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -471,12 +475,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2073324040"/>
+        <c:crossAx val="-2125170248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2073324040"/>
+        <c:axId val="-2125170248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -506,7 +510,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121396808"/>
+        <c:crossAx val="-2124918152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -653,11 +657,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2121330808"/>
-        <c:axId val="2121327816"/>
+        <c:axId val="2070533624"/>
+        <c:axId val="-2136853128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2121330808"/>
+        <c:axId val="2070533624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -667,12 +671,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121327816"/>
+        <c:crossAx val="-2136853128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2121327816"/>
+        <c:axId val="-2136853128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -683,7 +687,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121330808"/>
+        <c:crossAx val="2070533624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1087,10 +1091,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:Q16"/>
+  <dimension ref="B1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1792,17 +1796,57 @@
       <c r="H16" s="10">
         <v>10</v>
       </c>
-      <c r="I16" s="6"/>
+      <c r="I16" s="6">
+        <v>488</v>
+      </c>
       <c r="J16" s="3">
         <f t="shared" si="28"/>
         <v>72</v>
       </c>
       <c r="K16" s="7">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>6.7777777777777777</v>
       </c>
       <c r="L16">
         <f t="shared" si="30"/>
+        <v>720</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12">
+      <c r="B17" s="15">
+        <v>42687</v>
+      </c>
+      <c r="C17" s="1">
+        <v>900</v>
+      </c>
+      <c r="D17" s="1">
+        <v>2.1</v>
+      </c>
+      <c r="E17" s="10">
+        <v>2</v>
+      </c>
+      <c r="F17" s="10">
+        <v>36</v>
+      </c>
+      <c r="G17" s="10">
+        <v>10</v>
+      </c>
+      <c r="H17" s="10">
+        <v>10</v>
+      </c>
+      <c r="I17" s="6">
+        <v>233</v>
+      </c>
+      <c r="J17" s="3">
+        <f t="shared" ref="J17" si="31">F17*E17*G17/H17</f>
+        <v>72</v>
+      </c>
+      <c r="K17" s="7">
+        <f t="shared" ref="K17" si="32">I17/J17</f>
+        <v>3.2361111111111112</v>
+      </c>
+      <c r="L17">
+        <f t="shared" ref="L17" si="33">G17*F17*E17</f>
         <v>720</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update compute time records
</commit_message>
<xml_diff>
--- a/__cpttime.xlsx
+++ b/__cpttime.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="0" windowWidth="48000" windowHeight="27440" tabRatio="500"/>
+    <workbookView xWindow="1200" yWindow="620" windowWidth="25360" windowHeight="15820" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sherbrooke" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -154,7 +155,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Num intervention</t>
   </si>
@@ -209,15 +210,30 @@
   <si>
     <t>light output = TRUE ; peak memory = 1.9GB</t>
   </si>
+  <si>
+    <t>Wall time (minute)</t>
+  </si>
+  <si>
+    <t>Size output files (Gb)</t>
+  </si>
+  <si>
+    <t>Memory (Gb)</t>
+  </si>
+  <si>
+    <t>Earliest intervention</t>
+  </si>
+  <si>
+    <t>wall time / CPU (minute)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -305,6 +321,23 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -370,7 +403,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="75">
+  <cellStyleXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -446,8 +479,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -520,9 +569,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="75">
+  <cellStyles count="91">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -560,6 +633,14 @@
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -597,6 +678,14 @@
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -731,11 +820,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2147397800"/>
-        <c:axId val="-2135653400"/>
+        <c:axId val="2114389816"/>
+        <c:axId val="2114395032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2147397800"/>
+        <c:axId val="2114389816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -769,12 +858,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2135653400"/>
+        <c:crossAx val="2114395032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2135653400"/>
+        <c:axId val="2114395032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -804,7 +893,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2147397800"/>
+        <c:crossAx val="2114389816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -951,11 +1040,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2147210776"/>
-        <c:axId val="-2147053336"/>
+        <c:axId val="2114423032"/>
+        <c:axId val="2114426024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2147210776"/>
+        <c:axId val="2114423032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -965,12 +1054,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2147053336"/>
+        <c:crossAx val="2114426024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2147053336"/>
+        <c:axId val="2114426024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -981,7 +1070,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2147210776"/>
+        <c:crossAx val="2114423032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1088,11 +1177,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2140075544"/>
-        <c:axId val="-2140074920"/>
+        <c:axId val="2114448232"/>
+        <c:axId val="2114451320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2140075544"/>
+        <c:axId val="2114448232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1102,12 +1191,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140074920"/>
+        <c:crossAx val="2114451320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2140074920"/>
+        <c:axId val="2114451320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1118,7 +1207,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140075544"/>
+        <c:crossAx val="2114448232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1230,11 +1319,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2140364728"/>
-        <c:axId val="-2140575304"/>
+        <c:axId val="2114477672"/>
+        <c:axId val="2114480632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2140364728"/>
+        <c:axId val="2114477672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1244,12 +1333,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140575304"/>
+        <c:crossAx val="2114480632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2140575304"/>
+        <c:axId val="2114480632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.5"/>
@@ -1261,7 +1350,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140364728"/>
+        <c:crossAx val="2114477672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1732,8 +1821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:V28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
+    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2863,4 +2952,387 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.83203125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="5" customWidth="1"/>
+    <col min="9" max="10" width="15.5" style="5" customWidth="1"/>
+    <col min="11" max="11" width="38.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="30">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="9">
+        <v>42745</v>
+      </c>
+      <c r="B2" s="10">
+        <v>900</v>
+      </c>
+      <c r="C2" s="29">
+        <v>2</v>
+      </c>
+      <c r="D2" s="30">
+        <v>-2</v>
+      </c>
+      <c r="E2" s="29">
+        <v>24</v>
+      </c>
+      <c r="F2" s="29">
+        <v>24</v>
+      </c>
+      <c r="G2" s="31">
+        <v>3</v>
+      </c>
+      <c r="H2" s="32">
+        <v>3</v>
+      </c>
+      <c r="I2" s="32">
+        <v>0.4</v>
+      </c>
+      <c r="J2" s="36">
+        <f>G2*F2/E2</f>
+        <v>3</v>
+      </c>
+      <c r="K2" s="23"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="9">
+        <v>42745</v>
+      </c>
+      <c r="B3" s="15">
+        <v>300</v>
+      </c>
+      <c r="C3" s="30">
+        <v>2</v>
+      </c>
+      <c r="D3" s="30">
+        <v>-56</v>
+      </c>
+      <c r="E3" s="30">
+        <v>48</v>
+      </c>
+      <c r="F3" s="30">
+        <v>24</v>
+      </c>
+      <c r="G3" s="33">
+        <v>21</v>
+      </c>
+      <c r="H3" s="35">
+        <v>10</v>
+      </c>
+      <c r="I3" s="34">
+        <v>0.6</v>
+      </c>
+      <c r="J3" s="36">
+        <f>G3*F3/E3</f>
+        <v>10.5</v>
+      </c>
+      <c r="K3" s="25"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="9"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="25"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="9"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="25"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="9"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="25"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="9"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="25"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="9"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="25"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="9"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="25"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="9"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="25"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="9"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="25"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="9"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="25"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="9"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="25"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="9"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="25"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="9"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="25"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="9"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="25"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="9"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="25"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="9"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="25"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="9"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="25"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="9"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="25"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="9"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="25"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="9"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="25"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
start calculate average probability hosp
</commit_message>
<xml_diff>
--- a/__cpttime.xlsx
+++ b/__cpttime.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9960" yWindow="1520" windowWidth="35400" windowHeight="13940" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1700" yWindow="500" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -874,11 +874,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2116728296"/>
-        <c:axId val="-2140172040"/>
+        <c:axId val="2038675304"/>
+        <c:axId val="2038680968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2116728296"/>
+        <c:axId val="2038675304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -911,12 +911,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140172040"/>
+        <c:crossAx val="2038680968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2140172040"/>
+        <c:axId val="2038680968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -945,7 +945,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2116728296"/>
+        <c:crossAx val="2038675304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1092,11 +1092,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2140179208"/>
-        <c:axId val="-2114824648"/>
+        <c:axId val="2038538056"/>
+        <c:axId val="2038535064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2140179208"/>
+        <c:axId val="2038538056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1106,12 +1106,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114824648"/>
+        <c:crossAx val="2038535064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2114824648"/>
+        <c:axId val="2038535064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1122,7 +1122,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140179208"/>
+        <c:crossAx val="2038538056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1228,11 +1228,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2114802872"/>
-        <c:axId val="-2114799784"/>
+        <c:axId val="2088537016"/>
+        <c:axId val="2088539592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2114802872"/>
+        <c:axId val="2088537016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1242,12 +1242,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114799784"/>
+        <c:crossAx val="2088539592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2114799784"/>
+        <c:axId val="2088539592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1258,7 +1258,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2114802872"/>
+        <c:crossAx val="2088537016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1368,11 +1368,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2140246680"/>
-        <c:axId val="-2113953944"/>
+        <c:axId val="2039895304"/>
+        <c:axId val="2039892248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2140246680"/>
+        <c:axId val="2039895304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1382,12 +1382,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113953944"/>
+        <c:crossAx val="2039892248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2113953944"/>
+        <c:axId val="2039892248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.5"/>
@@ -1399,7 +1399,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2140246680"/>
+        <c:crossAx val="2039895304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1434,6 +1434,29 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Wall</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> time / CPU</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1504,7 +1527,7 @@
                   <c:v>0.954242509439325</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.929418925714293</c:v>
+                  <c:v>1.113943352306837</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1.698970004336019</c:v>
@@ -1522,11 +1545,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2115959736"/>
-        <c:axId val="-2123498760"/>
+        <c:axId val="2088562632"/>
+        <c:axId val="2088553720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2115959736"/>
+        <c:axId val="2088562632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1537,12 +1560,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123498760"/>
+        <c:crossAx val="2088553720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2123498760"/>
+        <c:axId val="2088553720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1553,7 +1576,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2115959736"/>
+        <c:crossAx val="2088562632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3191,8 +3214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3206,7 +3229,7 @@
     <col min="7" max="7" width="13.83203125" style="5" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" style="5" customWidth="1"/>
     <col min="9" max="10" width="15.5" style="5" customWidth="1"/>
-    <col min="11" max="11" width="38.83203125" customWidth="1"/>
+    <col min="11" max="11" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="30">
@@ -3382,13 +3405,17 @@
         <v>24</v>
       </c>
       <c r="G5" s="33">
-        <v>17</v>
-      </c>
-      <c r="H5" s="35"/>
-      <c r="I5" s="34"/>
+        <v>26</v>
+      </c>
+      <c r="H5" s="35">
+        <v>11</v>
+      </c>
+      <c r="I5" s="34">
+        <v>0.8</v>
+      </c>
       <c r="J5" s="36">
         <f t="shared" si="0"/>
-        <v>0.92941892571429274</v>
+        <v>1.1139433523068367</v>
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="37"/>

</xml_diff>